<commit_message>
Continued work on adding new variables
Added grouped siteID, TRT01P, TRT01A, TRT01PN, TRT01AN, and TRTDUR
</commit_message>
<xml_diff>
--- a/metadata/specs (1).xlsx
+++ b/metadata/specs (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagad\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucfi\Documents\Clinical Data\ClinicalExercise\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A111062A-78FB-4C24-94A4-656A686470F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E3AEF-F802-4341-9F00-AB3A92665EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7707" uniqueCount="1705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7723" uniqueCount="1706">
   <si>
     <t>Attribute</t>
   </si>
@@ -5434,12 +5434,15 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>X</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5537,6 +5540,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -5595,7 +5606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5631,16 +5642,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10020,7 +10029,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -11245,9 +11254,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S831"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F346" sqref="F346"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O235" sqref="O235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -18621,7 +18630,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="225" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="225" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A225" s="2" t="s">
         <v>187</v>
       </c>
@@ -18654,7 +18663,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="226" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="226" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A226" s="2" t="s">
         <v>190</v>
       </c>
@@ -18687,7 +18696,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="227" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="227" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A227" s="2" t="s">
         <v>193</v>
       </c>
@@ -18720,7 +18729,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="228" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="228" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A228" s="2" t="s">
         <v>196</v>
       </c>
@@ -18753,7 +18762,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="229" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="229" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A229" s="2" t="s">
         <v>300</v>
       </c>
@@ -18783,7 +18792,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="230" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="230" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A230" s="2" t="s">
         <v>304</v>
       </c>
@@ -18816,7 +18825,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="231" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="231" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A231" s="2" t="s">
         <v>308</v>
       </c>
@@ -18849,7 +18858,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="232" spans="1:15" ht="15.75" customHeight="1">
+    <row r="232" spans="1:19" ht="15.75" customHeight="1">
       <c r="A232" s="2" t="s">
         <v>64</v>
       </c>
@@ -18878,8 +18887,11 @@
       <c r="O232" s="2" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="233" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S232" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="233" spans="1:19" ht="15.75" customHeight="1">
       <c r="A233" s="2" t="s">
         <v>70</v>
       </c>
@@ -18908,8 +18920,11 @@
       <c r="O233" s="2" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="234" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S233" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="234" spans="1:19" ht="15.75" customHeight="1">
       <c r="A234" s="2" t="s">
         <v>73</v>
       </c>
@@ -18938,8 +18953,11 @@
       <c r="O234" s="2" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="235" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S234" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="235" spans="1:19" ht="15.75" customHeight="1">
       <c r="A235" s="2" t="s">
         <v>76</v>
       </c>
@@ -18968,8 +18986,11 @@
       <c r="O235" s="2" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="236" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S235" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="236" spans="1:19" ht="15.75" customHeight="1">
       <c r="A236" s="2" t="s">
         <v>79</v>
       </c>
@@ -18999,7 +19020,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="237" spans="1:15" ht="15.75" customHeight="1">
+    <row r="237" spans="1:19" ht="15.75" customHeight="1">
       <c r="A237" s="2" t="s">
         <v>85</v>
       </c>
@@ -19031,8 +19052,11 @@
       <c r="O237" s="2" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="238" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S237" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="238" spans="1:19" ht="15.75" customHeight="1">
       <c r="A238" s="2" t="s">
         <v>88</v>
       </c>
@@ -19065,7 +19089,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="239" spans="1:15" ht="15.75" customHeight="1">
+    <row r="239" spans="1:19" ht="15.75" customHeight="1">
       <c r="A239" s="2" t="s">
         <v>83</v>
       </c>
@@ -19098,7 +19122,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="240" spans="1:15" ht="15.75" customHeight="1">
+    <row r="240" spans="1:19" ht="15.75" customHeight="1">
       <c r="A240" s="2" t="s">
         <v>96</v>
       </c>
@@ -19131,7 +19155,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="241" spans="1:15" ht="15.75" customHeight="1">
+    <row r="241" spans="1:19" ht="15.75" customHeight="1">
       <c r="A241" s="2" t="s">
         <v>99</v>
       </c>
@@ -19164,7 +19188,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="242" spans="1:15" ht="15.75" customHeight="1">
+    <row r="242" spans="1:19" ht="15.75" customHeight="1">
       <c r="A242" s="2" t="s">
         <v>78</v>
       </c>
@@ -19196,8 +19220,11 @@
       <c r="O242" s="2" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="243" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S242" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="243" spans="1:19" ht="15.75" customHeight="1">
       <c r="A243" s="2" t="s">
         <v>68</v>
       </c>
@@ -19229,8 +19256,11 @@
       <c r="O243" s="2" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="244" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S243" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="244" spans="1:19" ht="15.75" customHeight="1">
       <c r="A244" s="2" t="s">
         <v>107</v>
       </c>
@@ -19260,7 +19290,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="245" spans="1:15" ht="15.75" customHeight="1">
+    <row r="245" spans="1:19" ht="15.75" customHeight="1">
       <c r="A245" s="2" t="s">
         <v>110</v>
       </c>
@@ -19293,7 +19323,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="246" spans="1:15" ht="15.75" customHeight="1">
+    <row r="246" spans="1:19" ht="15.75" customHeight="1">
       <c r="A246" s="2" t="s">
         <v>113</v>
       </c>
@@ -19326,7 +19356,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="247" spans="1:15" ht="15.75" customHeight="1">
+    <row r="247" spans="1:19" ht="15.75" customHeight="1">
       <c r="A247" s="2" t="s">
         <v>117</v>
       </c>
@@ -19355,8 +19385,11 @@
       <c r="O247" s="2" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="248" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S247" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="248" spans="1:19" ht="15.75" customHeight="1">
       <c r="A248" s="2" t="s">
         <v>120</v>
       </c>
@@ -19389,7 +19422,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="249" spans="1:15" ht="15.75" customHeight="1">
+    <row r="249" spans="1:19" ht="15.75" customHeight="1">
       <c r="A249" s="2" t="s">
         <v>123</v>
       </c>
@@ -19422,7 +19455,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="250" spans="1:15" ht="15.75" customHeight="1">
+    <row r="250" spans="1:19" ht="15.75" customHeight="1">
       <c r="A250" s="2" t="s">
         <v>126</v>
       </c>
@@ -19454,8 +19487,11 @@
       <c r="O250" s="2" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="251" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S250" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="251" spans="1:19" ht="15.75" customHeight="1">
       <c r="A251" s="2" t="s">
         <v>91</v>
       </c>
@@ -19487,8 +19523,11 @@
       <c r="O251" s="2" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="252" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S251" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="252" spans="1:19" ht="15.75" customHeight="1">
       <c r="A252" s="2" t="s">
         <v>131</v>
       </c>
@@ -19521,7 +19560,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="253" spans="1:15" ht="15.75" customHeight="1">
+    <row r="253" spans="1:19" ht="15.75" customHeight="1">
       <c r="A253" s="2" t="s">
         <v>135</v>
       </c>
@@ -19553,8 +19592,11 @@
       <c r="O253" s="2" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="254" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S253" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="254" spans="1:19" ht="15.75" customHeight="1">
       <c r="A254" s="2" t="s">
         <v>138</v>
       </c>
@@ -19586,8 +19628,11 @@
       <c r="O254" s="2" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="255" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S254" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="255" spans="1:19" ht="15.75" customHeight="1">
       <c r="A255" s="2" t="s">
         <v>141</v>
       </c>
@@ -19620,7 +19665,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="256" spans="1:15" ht="15.75" customHeight="1">
+    <row r="256" spans="1:19" ht="15.75" customHeight="1">
       <c r="A256" s="2" t="s">
         <v>147</v>
       </c>
@@ -19653,7 +19698,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="257" spans="1:15" ht="15.75" customHeight="1">
+    <row r="257" spans="1:19" ht="15.75" customHeight="1">
       <c r="A257" s="2" t="s">
         <v>151</v>
       </c>
@@ -19686,7 +19731,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="258" spans="1:15" ht="15.75" customHeight="1">
+    <row r="258" spans="1:19" ht="15.75" customHeight="1">
       <c r="A258" s="2" t="s">
         <v>155</v>
       </c>
@@ -19719,7 +19764,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="259" spans="1:15" ht="15.75" customHeight="1">
+    <row r="259" spans="1:19" ht="15.75" customHeight="1">
       <c r="A259" s="2" t="s">
         <v>159</v>
       </c>
@@ -19752,7 +19797,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="260" spans="1:15" ht="15.75" customHeight="1">
+    <row r="260" spans="1:19" ht="15.75" customHeight="1">
       <c r="A260" s="2" t="s">
         <v>162</v>
       </c>
@@ -19785,7 +19830,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="261" spans="1:15" ht="15.75" customHeight="1">
+    <row r="261" spans="1:19" ht="15.75" customHeight="1">
       <c r="A261" s="2" t="s">
         <v>165</v>
       </c>
@@ -19818,7 +19863,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="262" spans="1:15" ht="15.75" customHeight="1">
+    <row r="262" spans="1:19" ht="15.75" customHeight="1">
       <c r="A262" s="2" t="s">
         <v>168</v>
       </c>
@@ -19851,7 +19896,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="263" spans="1:15" ht="15.75" customHeight="1">
+    <row r="263" spans="1:19" ht="15.75" customHeight="1">
       <c r="A263" s="2" t="s">
         <v>106</v>
       </c>
@@ -19883,8 +19928,11 @@
       <c r="O263" s="2" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="264" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S263" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="264" spans="1:19" ht="15.75" customHeight="1">
       <c r="A264" s="2" t="s">
         <v>174</v>
       </c>
@@ -19917,7 +19965,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="265" spans="1:15" ht="15.75" customHeight="1">
+    <row r="265" spans="1:19" ht="15.75" customHeight="1">
       <c r="A265" s="2" t="s">
         <v>178</v>
       </c>
@@ -19950,7 +19998,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="266" spans="1:15" ht="15.75" customHeight="1">
+    <row r="266" spans="1:19" ht="15.75" customHeight="1">
       <c r="A266" s="2" t="s">
         <v>181</v>
       </c>
@@ -19983,7 +20031,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="267" spans="1:15" ht="15.75" customHeight="1">
+    <row r="267" spans="1:19" ht="15.75" customHeight="1">
       <c r="A267" s="2" t="s">
         <v>184</v>
       </c>
@@ -20016,7 +20064,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="268" spans="1:15" ht="15.75" customHeight="1">
+    <row r="268" spans="1:19" ht="15.75" customHeight="1">
       <c r="A268" s="2" t="s">
         <v>187</v>
       </c>
@@ -20046,7 +20094,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="269" spans="1:15" ht="15.75" customHeight="1">
+    <row r="269" spans="1:19" ht="15.75" customHeight="1">
       <c r="A269" s="2" t="s">
         <v>190</v>
       </c>
@@ -20079,7 +20127,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="270" spans="1:15" ht="15.75" customHeight="1">
+    <row r="270" spans="1:19" ht="15.75" customHeight="1">
       <c r="A270" s="2" t="s">
         <v>193</v>
       </c>
@@ -20112,7 +20160,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="271" spans="1:15" ht="15.75" customHeight="1">
+    <row r="271" spans="1:19" ht="15.75" customHeight="1">
       <c r="A271" s="2" t="s">
         <v>196</v>
       </c>
@@ -20145,7 +20193,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="272" spans="1:15" ht="15.75" customHeight="1">
+    <row r="272" spans="1:19" ht="15.75" customHeight="1">
       <c r="A272" s="2" t="s">
         <v>300</v>
       </c>
@@ -20178,7 +20226,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="273" spans="1:15" ht="15.75" customHeight="1">
+    <row r="273" spans="1:19" ht="15.75" customHeight="1">
       <c r="A273" s="2" t="s">
         <v>304</v>
       </c>
@@ -20207,8 +20255,12 @@
       <c r="O273" s="2" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="274" spans="1:15" ht="15.75" customHeight="1">
+      <c r="R273" s="24"/>
+      <c r="S273" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="274" spans="1:19" ht="15.75" customHeight="1">
       <c r="A274" s="2" t="s">
         <v>308</v>
       </c>
@@ -20237,8 +20289,12 @@
       <c r="O274" s="2" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="275" spans="1:15" ht="15.75" customHeight="1">
+      <c r="R274" s="24"/>
+      <c r="S274" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="275" spans="1:19" ht="15.75" customHeight="1">
       <c r="A275" s="2" t="s">
         <v>313</v>
       </c>
@@ -20268,7 +20324,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="276" spans="1:15" ht="15.75" customHeight="1">
+    <row r="276" spans="1:19" ht="15.75" customHeight="1">
       <c r="A276" s="2" t="s">
         <v>317</v>
       </c>
@@ -20300,8 +20356,11 @@
       <c r="O276" s="2" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="277" spans="1:15" ht="15.75" customHeight="1">
+      <c r="S276" s="24" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="277" spans="1:19" ht="15.75" customHeight="1">
       <c r="A277" s="2" t="s">
         <v>242</v>
       </c>
@@ -20334,7 +20393,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="278" spans="1:15" ht="15.75" customHeight="1">
+    <row r="278" spans="1:19" ht="15.75" customHeight="1">
       <c r="A278" s="2" t="s">
         <v>324</v>
       </c>
@@ -20364,7 +20423,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="279" spans="1:15" ht="15.75" customHeight="1">
+    <row r="279" spans="1:19" ht="15.75" customHeight="1">
       <c r="A279" s="2" t="s">
         <v>328</v>
       </c>
@@ -20397,7 +20456,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="280" spans="1:15" ht="15.75" customHeight="1">
+    <row r="280" spans="1:19" ht="15.75" customHeight="1">
       <c r="A280" s="2" t="s">
         <v>332</v>
       </c>
@@ -20427,7 +20486,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="281" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="281" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A281" s="2" t="s">
         <v>64</v>
       </c>
@@ -20457,7 +20516,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="282" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="282" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A282" s="2" t="s">
         <v>70</v>
       </c>
@@ -20487,7 +20546,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="283" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="283" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A283" s="2" t="s">
         <v>73</v>
       </c>
@@ -20517,7 +20576,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="284" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="284" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A284" s="2" t="s">
         <v>76</v>
       </c>
@@ -20547,7 +20606,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="285" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="285" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A285" s="2" t="s">
         <v>79</v>
       </c>
@@ -20580,7 +20639,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="286" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="286" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A286" s="2" t="s">
         <v>85</v>
       </c>
@@ -20613,7 +20672,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="287" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="287" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A287" s="2" t="s">
         <v>88</v>
       </c>
@@ -20646,7 +20705,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="288" spans="1:15" ht="15.75" hidden="1" customHeight="1">
+    <row r="288" spans="1:19" ht="15.75" hidden="1" customHeight="1">
       <c r="A288" s="2" t="s">
         <v>83</v>
       </c>
@@ -34280,7 +34339,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -35338,7 +35397,7 @@
   <dimension ref="A1:H790"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
@@ -35347,7 +35406,7 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="63.85546875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="63.85546875" customWidth="1"/>
     <col min="5" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
@@ -35364,7 +35423,7 @@
       <c r="C1" s="1" t="s">
         <v>1157</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="1" t="s">
         <v>1158</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -35548,7 +35607,7 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" hidden="1">
+    <row r="14" spans="1:8" ht="30" hidden="1">
       <c r="A14" s="2" t="s">
         <v>233</v>
       </c>
@@ -35968,7 +36027,7 @@
         <v>1242</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="105" hidden="1">
+    <row r="44" spans="1:4" ht="75" hidden="1">
       <c r="A44" s="2" t="s">
         <v>355</v>
       </c>
@@ -36286,7 +36345,7 @@
       <c r="C66" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="D66" s="12" t="s">
         <v>1274</v>
       </c>
     </row>
@@ -36300,11 +36359,11 @@
       <c r="C67" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D67" s="24" t="s">
+      <c r="D67" s="22" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="255">
+    <row r="68" spans="1:4" ht="195">
       <c r="A68" s="20" t="s">
         <v>427</v>
       </c>
@@ -36314,7 +36373,7 @@
       <c r="C68" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D68" s="24" t="s">
+      <c r="D68" s="22" t="s">
         <v>1700</v>
       </c>
     </row>
@@ -36342,7 +36401,7 @@
       <c r="C70" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D70" s="24" t="s">
+      <c r="D70" s="22" t="s">
         <v>125</v>
       </c>
     </row>
@@ -36356,7 +36415,7 @@
       <c r="C71" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="22" t="s">
         <v>1280</v>
       </c>
     </row>
@@ -37448,7 +37507,7 @@
       <c r="C149" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D149" s="22" t="s">
+      <c r="D149" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37462,7 +37521,7 @@
       <c r="C150" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D150" s="22" t="s">
+      <c r="D150" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37476,7 +37535,7 @@
       <c r="C151" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D151" s="22" t="s">
+      <c r="D151" s="21" t="s">
         <v>431</v>
       </c>
     </row>
@@ -37490,7 +37549,7 @@
       <c r="C152" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D152" s="22" t="s">
+      <c r="D152" s="21" t="s">
         <v>1265</v>
       </c>
     </row>
@@ -37504,7 +37563,7 @@
       <c r="C153" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D153" s="22" t="s">
+      <c r="D153" s="21" t="s">
         <v>1267</v>
       </c>
     </row>
@@ -37518,7 +37577,7 @@
       <c r="C154" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D154" s="22" t="s">
+      <c r="D154" s="21" t="s">
         <v>583</v>
       </c>
     </row>
@@ -37532,7 +37591,7 @@
       <c r="C155" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D155" s="22" t="s">
+      <c r="D155" s="21" t="s">
         <v>584</v>
       </c>
     </row>
@@ -37546,7 +37605,7 @@
       <c r="C156" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D156" s="22" t="s">
+      <c r="D156" s="21" t="s">
         <v>585</v>
       </c>
     </row>
@@ -37560,7 +37619,7 @@
       <c r="C157" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D157" s="22" t="s">
+      <c r="D157" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37574,7 +37633,7 @@
       <c r="C158" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D158" s="22" t="s">
+      <c r="D158" s="21" t="s">
         <v>125</v>
       </c>
     </row>
@@ -37588,7 +37647,7 @@
       <c r="C159" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D159" s="22" t="s">
+      <c r="D159" s="21" t="s">
         <v>1280</v>
       </c>
     </row>
@@ -37602,7 +37661,7 @@
       <c r="C160" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D160" s="22" t="s">
+      <c r="D160" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37616,7 +37675,7 @@
       <c r="C161" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D161" s="22" t="s">
+      <c r="D161" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37630,7 +37689,7 @@
       <c r="C162" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D162" s="22" t="s">
+      <c r="D162" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37644,7 +37703,7 @@
       <c r="C163" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D163" s="22" t="s">
+      <c r="D163" s="21" t="s">
         <v>605</v>
       </c>
     </row>
@@ -37658,7 +37717,7 @@
       <c r="C164" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D164" s="22" t="s">
+      <c r="D164" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37672,7 +37731,7 @@
       <c r="C165" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D165" s="22" t="s">
+      <c r="D165" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37686,7 +37745,7 @@
       <c r="C166" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D166" s="22" t="s">
+      <c r="D166" s="21" t="s">
         <v>1393</v>
       </c>
     </row>
@@ -37700,7 +37759,7 @@
       <c r="C167" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D167" s="22" t="s">
+      <c r="D167" s="21" t="s">
         <v>609</v>
       </c>
     </row>
@@ -37714,7 +37773,7 @@
       <c r="C168" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D168" s="22" t="s">
+      <c r="D168" s="21" t="s">
         <v>1396</v>
       </c>
     </row>
@@ -37728,7 +37787,7 @@
       <c r="C169" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D169" s="22" t="s">
+      <c r="D169" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37742,7 +37801,7 @@
       <c r="C170" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D170" s="22" t="s">
+      <c r="D170" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37756,7 +37815,7 @@
       <c r="C171" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D171" s="22" t="s">
+      <c r="D171" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37770,7 +37829,7 @@
       <c r="C172" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D172" s="22" t="s">
+      <c r="D172" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37784,7 +37843,7 @@
       <c r="C173" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D173" s="22" t="s">
+      <c r="D173" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37798,7 +37857,7 @@
       <c r="C174" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D174" s="22" t="s">
+      <c r="D174" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37812,7 +37871,7 @@
       <c r="C175" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D175" s="22" t="s">
+      <c r="D175" s="21" t="s">
         <v>589</v>
       </c>
     </row>
@@ -37826,7 +37885,7 @@
       <c r="C176" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D176" s="22" t="s">
+      <c r="D176" s="21" t="s">
         <v>590</v>
       </c>
     </row>
@@ -37840,7 +37899,7 @@
       <c r="C177" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D177" s="22" t="s">
+      <c r="D177" s="21" t="s">
         <v>595</v>
       </c>
     </row>
@@ -37854,7 +37913,7 @@
       <c r="C178" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D178" s="22" t="s">
+      <c r="D178" s="21" t="s">
         <v>591</v>
       </c>
     </row>
@@ -37868,7 +37927,7 @@
       <c r="C179" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D179" s="22" t="s">
+      <c r="D179" s="21" t="s">
         <v>1301</v>
       </c>
     </row>
@@ -37882,7 +37941,7 @@
       <c r="C180" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D180" s="22" t="s">
+      <c r="D180" s="21" t="s">
         <v>1409</v>
       </c>
     </row>
@@ -37896,7 +37955,7 @@
       <c r="C181" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D181" s="22" t="s">
+      <c r="D181" s="21" t="s">
         <v>553</v>
       </c>
     </row>
@@ -37910,7 +37969,7 @@
       <c r="C182" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D182" s="22" t="s">
+      <c r="D182" s="21" t="s">
         <v>555</v>
       </c>
     </row>
@@ -37924,7 +37983,7 @@
       <c r="C183" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D183" s="22" t="s">
+      <c r="D183" s="21" t="s">
         <v>568</v>
       </c>
     </row>
@@ -37938,7 +37997,7 @@
       <c r="C184" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D184" s="22" t="s">
+      <c r="D184" s="21" t="s">
         <v>571</v>
       </c>
     </row>
@@ -37952,7 +38011,7 @@
       <c r="C185" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D185" s="22" t="s">
+      <c r="D185" s="21" t="s">
         <v>573</v>
       </c>
     </row>
@@ -37966,7 +38025,7 @@
       <c r="C186" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D186" s="22" t="s">
+      <c r="D186" s="21" t="s">
         <v>562</v>
       </c>
     </row>
@@ -37980,7 +38039,7 @@
       <c r="C187" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D187" s="22" t="s">
+      <c r="D187" s="21" t="s">
         <v>565</v>
       </c>
     </row>
@@ -37994,7 +38053,7 @@
       <c r="C188" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D188" s="22" t="s">
+      <c r="D188" s="21" t="s">
         <v>572</v>
       </c>
     </row>
@@ -38008,7 +38067,7 @@
       <c r="C189" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D189" s="22" t="s">
+      <c r="D189" s="21" t="s">
         <v>554</v>
       </c>
     </row>
@@ -38022,7 +38081,7 @@
       <c r="C190" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D190" s="22" t="s">
+      <c r="D190" s="21" t="s">
         <v>1306</v>
       </c>
     </row>
@@ -38036,7 +38095,7 @@
       <c r="C191" s="2" t="s">
         <v>1162</v>
       </c>
-      <c r="D191" s="22" t="s">
+      <c r="D191" s="21" t="s">
         <v>1307</v>
       </c>
     </row>
@@ -38194,7 +38253,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="180" hidden="1">
+    <row r="203" spans="1:4" ht="135" hidden="1">
       <c r="A203" s="2" t="s">
         <v>582</v>
       </c>
@@ -38698,7 +38757,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="60" hidden="1">
+    <row r="239" spans="1:4" ht="45" hidden="1">
       <c r="A239" s="2" t="s">
         <v>650</v>
       </c>
@@ -40336,7 +40395,7 @@
       <c r="E2" s="9" t="s">
         <v>1441</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="23" t="s">
         <v>1701</v>
       </c>
       <c r="G2" s="8"/>

</xml_diff>

<commit_message>
Comparison version of ADSL_LF
Rewrote ADSL.SAS.
</commit_message>
<xml_diff>
--- a/metadata/specs (1).xlsx
+++ b/metadata/specs (1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucfi\Documents\Clinical Data\ClinicalExercise\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1E3AEF-F802-4341-9F00-AB3A92665EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E967F5B6-F3A1-4E29-8183-44378B33580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11745" yWindow="4065" windowWidth="11250" windowHeight="10755" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -11254,9 +11254,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:S831"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A232" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O235" sqref="O235"/>
+      <selection pane="bottomLeft" activeCell="K239" sqref="K239"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -24034,11 +24034,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H955"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B170" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H251" sqref="H251"/>
+      <selection pane="bottomRight" activeCell="D492" sqref="D492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -24357,7 +24357,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>92</v>
       </c>
@@ -24377,7 +24377,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="17" spans="1:8" hidden="1">
+    <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>92</v>
       </c>
@@ -24397,7 +24397,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1">
+    <row r="18" spans="1:8">
       <c r="A18" s="2" t="s">
         <v>92</v>
       </c>
@@ -24417,7 +24417,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
         <v>95</v>
       </c>
@@ -24437,7 +24437,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1">
+    <row r="20" spans="1:8">
       <c r="A20" s="2" t="s">
         <v>95</v>
       </c>
@@ -24457,7 +24457,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" hidden="1" customHeight="1">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>95</v>
       </c>
@@ -26757,7 +26757,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="15.75" customHeight="1">
+    <row r="136" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A136" s="2" t="s">
         <v>469</v>
       </c>
@@ -26777,7 +26777,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="15.75" customHeight="1">
+    <row r="137" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A137" s="2" t="s">
         <v>469</v>
       </c>
@@ -26797,7 +26797,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="15.75" customHeight="1">
+    <row r="138" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A138" s="2" t="s">
         <v>469</v>
       </c>
@@ -26817,7 +26817,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="15.75" customHeight="1">
+    <row r="139" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A139" s="2" t="s">
         <v>469</v>
       </c>
@@ -26837,7 +26837,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="15.75" customHeight="1">
+    <row r="140" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A140" s="2" t="s">
         <v>469</v>
       </c>
@@ -26857,7 +26857,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="141" spans="1:8" ht="15.75" customHeight="1">
+    <row r="141" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A141" s="2" t="s">
         <v>469</v>
       </c>
@@ -26877,7 +26877,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="15.75" customHeight="1">
+    <row r="142" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A142" s="2" t="s">
         <v>469</v>
       </c>
@@ -26897,7 +26897,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="143" spans="1:8" ht="15.75" customHeight="1">
+    <row r="143" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A143" s="2" t="s">
         <v>469</v>
       </c>
@@ -26917,7 +26917,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="15.75" customHeight="1">
+    <row r="144" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A144" s="2" t="s">
         <v>469</v>
       </c>
@@ -26937,7 +26937,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="15.75" customHeight="1">
+    <row r="145" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A145" s="2" t="s">
         <v>469</v>
       </c>
@@ -26957,7 +26957,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="15.75" customHeight="1">
+    <row r="146" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A146" s="2" t="s">
         <v>469</v>
       </c>
@@ -26977,7 +26977,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="147" spans="1:8" ht="15.75" customHeight="1">
+    <row r="147" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A147" s="2" t="s">
         <v>469</v>
       </c>
@@ -26997,7 +26997,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="15.75" customHeight="1">
+    <row r="148" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A148" s="2" t="s">
         <v>469</v>
       </c>
@@ -27017,7 +27017,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="15.75" customHeight="1">
+    <row r="149" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A149" s="2" t="s">
         <v>469</v>
       </c>
@@ -27037,7 +27037,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="150" spans="1:8" ht="15.75" customHeight="1">
+    <row r="150" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A150" s="2" t="s">
         <v>469</v>
       </c>
@@ -27057,7 +27057,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="151" spans="1:8" ht="15.75" customHeight="1">
+    <row r="151" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A151" s="2" t="s">
         <v>469</v>
       </c>
@@ -27077,7 +27077,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="15.75" customHeight="1">
+    <row r="152" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A152" s="2" t="s">
         <v>469</v>
       </c>
@@ -27097,7 +27097,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="153" spans="1:8" ht="15.75" customHeight="1">
+    <row r="153" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A153" s="2" t="s">
         <v>469</v>
       </c>
@@ -27117,7 +27117,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="15.75" customHeight="1">
+    <row r="154" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A154" s="2" t="s">
         <v>469</v>
       </c>
@@ -27137,7 +27137,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="155" spans="1:8" ht="15.75" customHeight="1">
+    <row r="155" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A155" s="2" t="s">
         <v>469</v>
       </c>
@@ -27157,7 +27157,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="15.75" customHeight="1">
+    <row r="156" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A156" s="2" t="s">
         <v>469</v>
       </c>
@@ -27177,7 +27177,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="15.75" customHeight="1">
+    <row r="157" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A157" s="2" t="s">
         <v>469</v>
       </c>
@@ -27197,7 +27197,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="15.75" customHeight="1">
+    <row r="158" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A158" s="2" t="s">
         <v>469</v>
       </c>
@@ -27217,7 +27217,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="15.75" customHeight="1">
+    <row r="159" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A159" s="2" t="s">
         <v>469</v>
       </c>
@@ -27237,7 +27237,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="15.75" customHeight="1">
+    <row r="160" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A160" s="2" t="s">
         <v>469</v>
       </c>
@@ -27257,7 +27257,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="15.75" customHeight="1">
+    <row r="161" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A161" s="2" t="s">
         <v>469</v>
       </c>
@@ -27277,7 +27277,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="15.75" customHeight="1">
+    <row r="162" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A162" s="2" t="s">
         <v>469</v>
       </c>
@@ -27297,7 +27297,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="163" spans="1:8" ht="15.75" customHeight="1">
+    <row r="163" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A163" s="2" t="s">
         <v>469</v>
       </c>
@@ -27317,7 +27317,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="164" spans="1:8" ht="15.75" customHeight="1">
+    <row r="164" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A164" s="2" t="s">
         <v>469</v>
       </c>
@@ -27337,7 +27337,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="165" spans="1:8" ht="15.75" customHeight="1">
+    <row r="165" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A165" s="2" t="s">
         <v>469</v>
       </c>
@@ -27357,7 +27357,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="166" spans="1:8" ht="15.75" customHeight="1">
+    <row r="166" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A166" s="2" t="s">
         <v>469</v>
       </c>
@@ -27377,7 +27377,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="167" spans="1:8" ht="15.75" customHeight="1">
+    <row r="167" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A167" s="2" t="s">
         <v>469</v>
       </c>
@@ -27397,7 +27397,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="168" spans="1:8" ht="15.75" customHeight="1">
+    <row r="168" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A168" s="2" t="s">
         <v>469</v>
       </c>
@@ -27417,7 +27417,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="169" spans="1:8" ht="15.75" customHeight="1">
+    <row r="169" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A169" s="2" t="s">
         <v>469</v>
       </c>
@@ -27437,7 +27437,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="170" spans="1:8" ht="15.75" customHeight="1">
+    <row r="170" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A170" s="2" t="s">
         <v>521</v>
       </c>
@@ -27457,7 +27457,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="171" spans="1:8" ht="15.75" customHeight="1">
+    <row r="171" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A171" s="2" t="s">
         <v>521</v>
       </c>
@@ -27477,7 +27477,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="172" spans="1:8" ht="15.75" customHeight="1">
+    <row r="172" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A172" s="2" t="s">
         <v>521</v>
       </c>
@@ -27497,7 +27497,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="173" spans="1:8" ht="15.75" customHeight="1">
+    <row r="173" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A173" s="2" t="s">
         <v>521</v>
       </c>
@@ -27517,7 +27517,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="174" spans="1:8" ht="15.75" customHeight="1">
+    <row r="174" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A174" s="2" t="s">
         <v>521</v>
       </c>
@@ -27537,7 +27537,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="175" spans="1:8" ht="15.75" customHeight="1">
+    <row r="175" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A175" s="2" t="s">
         <v>521</v>
       </c>
@@ -28717,7 +28717,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="234" spans="1:8" ht="15.75" customHeight="1">
+    <row r="234" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A234" s="2" t="s">
         <v>471</v>
       </c>
@@ -28737,7 +28737,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="235" spans="1:8" ht="15.75" customHeight="1">
+    <row r="235" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A235" s="2" t="s">
         <v>471</v>
       </c>
@@ -28757,7 +28757,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="236" spans="1:8" ht="15.75" customHeight="1">
+    <row r="236" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A236" s="2" t="s">
         <v>471</v>
       </c>
@@ -28777,7 +28777,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="237" spans="1:8" ht="15.75" customHeight="1">
+    <row r="237" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A237" s="2" t="s">
         <v>471</v>
       </c>
@@ -28797,7 +28797,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="238" spans="1:8" ht="15.75" customHeight="1">
+    <row r="238" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A238" s="2" t="s">
         <v>471</v>
       </c>
@@ -28817,7 +28817,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="239" spans="1:8" ht="15.75" customHeight="1">
+    <row r="239" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A239" s="2" t="s">
         <v>471</v>
       </c>
@@ -28837,7 +28837,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="240" spans="1:8" ht="15.75" customHeight="1">
+    <row r="240" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A240" s="2" t="s">
         <v>471</v>
       </c>
@@ -28857,7 +28857,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="241" spans="1:8" ht="15.75" customHeight="1">
+    <row r="241" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A241" s="2" t="s">
         <v>471</v>
       </c>
@@ -28877,7 +28877,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="242" spans="1:8" ht="15.75" customHeight="1">
+    <row r="242" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A242" s="2" t="s">
         <v>471</v>
       </c>
@@ -28897,7 +28897,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="243" spans="1:8" ht="15.75" customHeight="1">
+    <row r="243" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A243" s="2" t="s">
         <v>471</v>
       </c>
@@ -28917,7 +28917,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="244" spans="1:8" ht="15.75" customHeight="1">
+    <row r="244" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A244" s="2" t="s">
         <v>471</v>
       </c>
@@ -28937,7 +28937,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="245" spans="1:8" ht="15.75" customHeight="1">
+    <row r="245" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A245" s="2" t="s">
         <v>471</v>
       </c>
@@ -28957,7 +28957,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="246" spans="1:8" ht="15.75" customHeight="1">
+    <row r="246" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A246" s="2" t="s">
         <v>471</v>
       </c>
@@ -28977,7 +28977,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="247" spans="1:8" ht="15.75" customHeight="1">
+    <row r="247" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A247" s="2" t="s">
         <v>471</v>
       </c>
@@ -28997,7 +28997,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="248" spans="1:8" ht="15.75" customHeight="1">
+    <row r="248" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A248" s="2" t="s">
         <v>471</v>
       </c>
@@ -29017,7 +29017,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="249" spans="1:8" ht="15.75" customHeight="1">
+    <row r="249" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A249" s="2" t="s">
         <v>471</v>
       </c>
@@ -29037,7 +29037,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="250" spans="1:8" ht="15.75" customHeight="1">
+    <row r="250" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A250" s="2" t="s">
         <v>471</v>
       </c>
@@ -29057,7 +29057,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="251" spans="1:8" ht="15.75" customHeight="1">
+    <row r="251" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A251" s="2" t="s">
         <v>471</v>
       </c>
@@ -29077,7 +29077,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="252" spans="1:8" ht="15.75" customHeight="1">
+    <row r="252" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A252" s="2" t="s">
         <v>471</v>
       </c>
@@ -29097,7 +29097,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="253" spans="1:8" ht="15.75" customHeight="1">
+    <row r="253" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A253" s="2" t="s">
         <v>471</v>
       </c>
@@ -29117,7 +29117,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="254" spans="1:8" ht="15.75" customHeight="1">
+    <row r="254" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A254" s="2" t="s">
         <v>471</v>
       </c>
@@ -29137,7 +29137,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="255" spans="1:8" ht="15.75" customHeight="1">
+    <row r="255" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A255" s="2" t="s">
         <v>471</v>
       </c>
@@ -29157,7 +29157,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="256" spans="1:8" ht="15.75" customHeight="1">
+    <row r="256" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A256" s="2" t="s">
         <v>471</v>
       </c>
@@ -29177,7 +29177,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="257" spans="1:8" ht="15.75" customHeight="1">
+    <row r="257" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A257" s="2" t="s">
         <v>471</v>
       </c>
@@ -29197,7 +29197,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="258" spans="1:8" ht="15.75" customHeight="1">
+    <row r="258" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A258" s="2" t="s">
         <v>471</v>
       </c>
@@ -29217,7 +29217,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="259" spans="1:8" ht="15.75" customHeight="1">
+    <row r="259" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A259" s="2" t="s">
         <v>471</v>
       </c>
@@ -29237,7 +29237,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="260" spans="1:8" ht="15.75" customHeight="1">
+    <row r="260" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A260" s="2" t="s">
         <v>471</v>
       </c>
@@ -29257,7 +29257,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="261" spans="1:8" ht="15.75" customHeight="1">
+    <row r="261" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A261" s="2" t="s">
         <v>471</v>
       </c>
@@ -29277,7 +29277,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="262" spans="1:8" ht="15.75" customHeight="1">
+    <row r="262" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A262" s="2" t="s">
         <v>471</v>
       </c>
@@ -29297,7 +29297,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="263" spans="1:8" ht="15.75" customHeight="1">
+    <row r="263" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A263" s="2" t="s">
         <v>471</v>
       </c>
@@ -29317,7 +29317,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="264" spans="1:8" ht="15.75" customHeight="1">
+    <row r="264" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A264" s="2" t="s">
         <v>471</v>
       </c>
@@ -29337,7 +29337,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="265" spans="1:8" ht="15.75" customHeight="1">
+    <row r="265" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A265" s="2" t="s">
         <v>471</v>
       </c>
@@ -29357,7 +29357,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="266" spans="1:8" ht="15.75" customHeight="1">
+    <row r="266" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A266" s="2" t="s">
         <v>471</v>
       </c>
@@ -29377,7 +29377,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="267" spans="1:8" ht="15.75" customHeight="1">
+    <row r="267" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A267" s="2" t="s">
         <v>471</v>
       </c>
@@ -29397,7 +29397,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="268" spans="1:8" ht="15.75" customHeight="1">
+    <row r="268" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A268" s="2" t="s">
         <v>523</v>
       </c>
@@ -29417,7 +29417,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="269" spans="1:8" ht="15.75" customHeight="1">
+    <row r="269" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A269" s="2" t="s">
         <v>523</v>
       </c>
@@ -29437,7 +29437,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="270" spans="1:8" ht="15.75" customHeight="1">
+    <row r="270" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A270" s="2" t="s">
         <v>523</v>
       </c>
@@ -29457,7 +29457,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="271" spans="1:8" ht="15.75" customHeight="1">
+    <row r="271" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A271" s="2" t="s">
         <v>523</v>
       </c>
@@ -29477,7 +29477,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="272" spans="1:8" ht="15.75" customHeight="1">
+    <row r="272" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A272" s="2" t="s">
         <v>523</v>
       </c>
@@ -29497,7 +29497,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="15.75" customHeight="1">
+    <row r="273" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A273" s="2" t="s">
         <v>523</v>
       </c>
@@ -30677,7 +30677,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="332" spans="1:8" ht="15.75" customHeight="1">
+    <row r="332" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A332" s="2" t="s">
         <v>467</v>
       </c>
@@ -30697,7 +30697,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="333" spans="1:8" ht="15.75" customHeight="1">
+    <row r="333" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A333" s="2" t="s">
         <v>467</v>
       </c>
@@ -30717,7 +30717,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="334" spans="1:8" ht="15.75" customHeight="1">
+    <row r="334" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A334" s="2" t="s">
         <v>467</v>
       </c>
@@ -30737,7 +30737,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="335" spans="1:8" ht="15.75" customHeight="1">
+    <row r="335" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A335" s="2" t="s">
         <v>467</v>
       </c>
@@ -30757,7 +30757,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="336" spans="1:8" ht="15.75" customHeight="1">
+    <row r="336" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A336" s="2" t="s">
         <v>467</v>
       </c>
@@ -30777,7 +30777,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="337" spans="1:8" ht="15.75" customHeight="1">
+    <row r="337" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A337" s="2" t="s">
         <v>467</v>
       </c>
@@ -30797,7 +30797,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="338" spans="1:8" ht="15.75" customHeight="1">
+    <row r="338" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A338" s="2" t="s">
         <v>467</v>
       </c>
@@ -30817,7 +30817,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="339" spans="1:8" ht="15.75" customHeight="1">
+    <row r="339" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A339" s="2" t="s">
         <v>467</v>
       </c>
@@ -30837,7 +30837,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="340" spans="1:8" ht="15.75" customHeight="1">
+    <row r="340" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A340" s="2" t="s">
         <v>467</v>
       </c>
@@ -30857,7 +30857,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="341" spans="1:8" ht="15.75" customHeight="1">
+    <row r="341" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A341" s="2" t="s">
         <v>467</v>
       </c>
@@ -30877,7 +30877,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="342" spans="1:8" ht="15.75" customHeight="1">
+    <row r="342" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A342" s="2" t="s">
         <v>467</v>
       </c>
@@ -30897,7 +30897,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="343" spans="1:8" ht="15.75" customHeight="1">
+    <row r="343" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A343" s="2" t="s">
         <v>467</v>
       </c>
@@ -30917,7 +30917,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="344" spans="1:8" ht="15.75" customHeight="1">
+    <row r="344" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A344" s="2" t="s">
         <v>467</v>
       </c>
@@ -30937,7 +30937,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="345" spans="1:8" ht="15.75" customHeight="1">
+    <row r="345" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A345" s="2" t="s">
         <v>467</v>
       </c>
@@ -30957,7 +30957,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="346" spans="1:8" ht="15.75" customHeight="1">
+    <row r="346" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A346" s="2" t="s">
         <v>467</v>
       </c>
@@ -30977,7 +30977,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="347" spans="1:8" ht="15.75" customHeight="1">
+    <row r="347" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A347" s="2" t="s">
         <v>467</v>
       </c>
@@ -30997,7 +30997,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="348" spans="1:8" ht="15.75" customHeight="1">
+    <row r="348" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A348" s="2" t="s">
         <v>467</v>
       </c>
@@ -31017,7 +31017,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="349" spans="1:8" ht="15.75" customHeight="1">
+    <row r="349" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A349" s="2" t="s">
         <v>467</v>
       </c>
@@ -31037,7 +31037,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="350" spans="1:8" ht="15.75" customHeight="1">
+    <row r="350" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A350" s="2" t="s">
         <v>467</v>
       </c>
@@ -31057,7 +31057,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="351" spans="1:8" ht="15.75" customHeight="1">
+    <row r="351" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A351" s="2" t="s">
         <v>467</v>
       </c>
@@ -31077,7 +31077,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="352" spans="1:8" ht="15.75" customHeight="1">
+    <row r="352" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A352" s="2" t="s">
         <v>467</v>
       </c>
@@ -31097,7 +31097,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="353" spans="1:8" ht="15.75" customHeight="1">
+    <row r="353" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A353" s="2" t="s">
         <v>467</v>
       </c>
@@ -31117,7 +31117,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="354" spans="1:8" ht="15.75" customHeight="1">
+    <row r="354" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A354" s="2" t="s">
         <v>467</v>
       </c>
@@ -31137,7 +31137,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="355" spans="1:8" ht="15.75" customHeight="1">
+    <row r="355" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A355" s="2" t="s">
         <v>467</v>
       </c>
@@ -31157,7 +31157,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="356" spans="1:8" ht="15.75" customHeight="1">
+    <row r="356" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A356" s="2" t="s">
         <v>467</v>
       </c>
@@ -31177,7 +31177,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="357" spans="1:8" ht="15.75" customHeight="1">
+    <row r="357" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A357" s="2" t="s">
         <v>467</v>
       </c>
@@ -31197,7 +31197,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="358" spans="1:8" ht="15.75" customHeight="1">
+    <row r="358" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A358" s="2" t="s">
         <v>467</v>
       </c>
@@ -31217,7 +31217,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="359" spans="1:8" ht="15.75" customHeight="1">
+    <row r="359" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A359" s="2" t="s">
         <v>467</v>
       </c>
@@ -31237,7 +31237,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="360" spans="1:8" ht="15.75" customHeight="1">
+    <row r="360" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A360" s="2" t="s">
         <v>467</v>
       </c>
@@ -31257,7 +31257,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="361" spans="1:8" ht="15.75" customHeight="1">
+    <row r="361" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A361" s="2" t="s">
         <v>467</v>
       </c>
@@ -31277,7 +31277,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="362" spans="1:8" ht="15.75" customHeight="1">
+    <row r="362" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A362" s="2" t="s">
         <v>467</v>
       </c>
@@ -31297,7 +31297,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="363" spans="1:8" ht="15.75" customHeight="1">
+    <row r="363" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A363" s="2" t="s">
         <v>467</v>
       </c>
@@ -31317,7 +31317,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="364" spans="1:8" ht="15.75" customHeight="1">
+    <row r="364" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A364" s="2" t="s">
         <v>467</v>
       </c>
@@ -31337,7 +31337,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="365" spans="1:8" ht="15.75" customHeight="1">
+    <row r="365" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A365" s="2" t="s">
         <v>467</v>
       </c>
@@ -31357,7 +31357,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="366" spans="1:8" ht="15.75" customHeight="1">
+    <row r="366" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A366" s="2" t="s">
         <v>519</v>
       </c>
@@ -31377,7 +31377,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="367" spans="1:8" ht="15.75" customHeight="1">
+    <row r="367" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A367" s="2" t="s">
         <v>519</v>
       </c>
@@ -31397,7 +31397,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="368" spans="1:8" ht="15.75" customHeight="1">
+    <row r="368" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A368" s="2" t="s">
         <v>519</v>
       </c>
@@ -31417,7 +31417,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="369" spans="1:8" ht="15.75" customHeight="1">
+    <row r="369" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A369" s="2" t="s">
         <v>519</v>
       </c>
@@ -31437,7 +31437,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="370" spans="1:8" ht="15.75" customHeight="1">
+    <row r="370" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A370" s="2" t="s">
         <v>519</v>
       </c>
@@ -31457,7 +31457,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="371" spans="1:8" ht="15.75" customHeight="1">
+    <row r="371" spans="1:8" ht="15.75" hidden="1" customHeight="1">
       <c r="A371" s="2" t="s">
         <v>519</v>
       </c>
@@ -34314,12 +34314,8 @@
   <autoFilter ref="A1:H490" xr:uid="{00000000-0009-0000-0000-000004000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="PARAM_ADLBH"/>
-        <filter val="PARAM_ADLBHY"/>
-        <filter val="PARAMCD_ADLBH"/>
-        <filter val="PARAMCD_ADLBHY"/>
-        <filter val="PARAMN_ADLBH"/>
-        <filter val="PARAMN_ADLBHY"/>
+        <filter val="ARM"/>
+        <filter val="ARMN"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -35397,8 +35393,8 @@
   <dimension ref="A1:H790"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D203" sqref="D203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -36209,7 +36205,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+    <row r="57" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A57" s="2" t="s">
         <v>407</v>
       </c>
@@ -36223,7 +36219,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+    <row r="58" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A58" s="2" t="s">
         <v>404</v>
       </c>
@@ -36237,7 +36233,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1">
+    <row r="59" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A59" s="2" t="s">
         <v>431</v>
       </c>
@@ -36251,7 +36247,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1">
+    <row r="60" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A60" s="2" t="s">
         <v>386</v>
       </c>
@@ -36265,7 +36261,7 @@
         <v>1265</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+    <row r="61" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A61" s="2" t="s">
         <v>385</v>
       </c>
@@ -36279,7 +36275,7 @@
         <v>1267</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1">
+    <row r="62" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A62" s="20" t="s">
         <v>434</v>
       </c>
@@ -36293,7 +36289,7 @@
         <v>1269</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1">
+    <row r="63" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A63" s="2" t="s">
         <v>372</v>
       </c>
@@ -36307,7 +36303,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1">
+    <row r="64" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A64" s="2" t="s">
         <v>373</v>
       </c>
@@ -36321,7 +36317,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" customHeight="1">
+    <row r="65" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A65" s="2" t="s">
         <v>374</v>
       </c>
@@ -36335,7 +36331,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1">
+    <row r="66" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A66" s="20" t="s">
         <v>423</v>
       </c>
@@ -36349,7 +36345,7 @@
         <v>1274</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1">
+    <row r="67" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="2" t="s">
         <v>420</v>
       </c>
@@ -36363,7 +36359,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="195">
+    <row r="68" spans="1:4" ht="195" hidden="1">
       <c r="A68" s="20" t="s">
         <v>427</v>
       </c>
@@ -36377,7 +36373,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1">
+    <row r="69" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="2" t="s">
         <v>399</v>
       </c>
@@ -36391,7 +36387,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" customHeight="1">
+    <row r="70" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A70" s="2" t="s">
         <v>383</v>
       </c>
@@ -36405,7 +36401,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" customHeight="1">
+    <row r="71" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="2" t="s">
         <v>384</v>
       </c>
@@ -36419,7 +36415,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" customHeight="1">
+    <row r="72" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A72" s="2" t="s">
         <v>400</v>
       </c>
@@ -36433,7 +36429,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" customHeight="1">
+    <row r="73" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="2" t="s">
         <v>430</v>
       </c>
@@ -36447,7 +36443,7 @@
         <v>1698</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" customHeight="1">
+    <row r="74" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A74" s="2" t="s">
         <v>419</v>
       </c>
@@ -36461,7 +36457,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" customHeight="1">
+    <row r="75" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A75" s="20" t="s">
         <v>416</v>
       </c>
@@ -36475,7 +36471,7 @@
         <v>1286</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" customHeight="1">
+    <row r="76" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A76" s="2" t="s">
         <v>401</v>
       </c>
@@ -36489,7 +36485,7 @@
         <v>1696</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" customHeight="1">
+    <row r="77" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A77" s="2" t="s">
         <v>378</v>
       </c>
@@ -36503,7 +36499,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" customHeight="1">
+    <row r="78" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A78" s="2" t="s">
         <v>381</v>
       </c>
@@ -36517,7 +36513,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" customHeight="1">
+    <row r="79" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A79" s="2" t="s">
         <v>439</v>
       </c>
@@ -36531,7 +36527,7 @@
         <v>1291</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" customHeight="1">
+    <row r="80" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A80" s="2" t="s">
         <v>436</v>
       </c>
@@ -36545,7 +36541,7 @@
         <v>1293</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" customHeight="1">
+    <row r="81" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A81" s="2" t="s">
         <v>442</v>
       </c>
@@ -36559,7 +36555,7 @@
         <v>1295</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.75" customHeight="1">
+    <row r="82" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A82" s="2" t="s">
         <v>390</v>
       </c>
@@ -36573,7 +36569,7 @@
         <v>1297</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.75" customHeight="1">
+    <row r="83" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A83" s="2" t="s">
         <v>392</v>
       </c>
@@ -36587,7 +36583,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" customHeight="1">
+    <row r="84" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A84" s="2" t="s">
         <v>394</v>
       </c>
@@ -36601,7 +36597,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.75" customHeight="1">
+    <row r="85" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A85" s="2" t="s">
         <v>398</v>
       </c>
@@ -36615,7 +36611,7 @@
         <v>1697</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.75" customHeight="1">
+    <row r="86" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A86" s="2" t="s">
         <v>413</v>
       </c>
@@ -36629,7 +36625,7 @@
         <v>1304</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" customHeight="1">
+    <row r="87" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A87" s="20" t="s">
         <v>410</v>
       </c>
@@ -36643,7 +36639,7 @@
         <v>1305</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" customHeight="1">
+    <row r="88" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A88" s="2" t="s">
         <v>375</v>
       </c>
@@ -36657,7 +36653,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" customHeight="1">
+    <row r="89" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A89" s="2" t="s">
         <v>376</v>
       </c>
@@ -36671,7 +36667,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" customHeight="1">
+    <row r="90" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A90" s="2" t="s">
         <v>382</v>
       </c>
@@ -36685,7 +36681,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" customHeight="1">
+    <row r="91" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A91" s="2" t="s">
         <v>377</v>
       </c>
@@ -36699,7 +36695,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.75" customHeight="1">
+    <row r="92" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A92" s="2" t="s">
         <v>361</v>
       </c>
@@ -36713,7 +36709,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.75" customHeight="1">
+    <row r="93" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A93" s="2" t="s">
         <v>364</v>
       </c>
@@ -36727,7 +36723,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" customHeight="1">
+    <row r="94" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A94" s="2" t="s">
         <v>368</v>
       </c>
@@ -36741,7 +36737,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" customHeight="1">
+    <row r="95" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A95" s="2" t="s">
         <v>369</v>
       </c>
@@ -36755,7 +36751,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" customHeight="1">
+    <row r="96" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A96" s="2" t="s">
         <v>371</v>
       </c>
@@ -36769,7 +36765,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" customHeight="1">
+    <row r="97" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A97" s="2" t="s">
         <v>366</v>
       </c>
@@ -36783,7 +36779,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.75" customHeight="1">
+    <row r="98" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A98" s="2" t="s">
         <v>367</v>
       </c>
@@ -36797,7 +36793,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.75" customHeight="1">
+    <row r="99" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A99" s="2" t="s">
         <v>370</v>
       </c>
@@ -36811,7 +36807,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.75" customHeight="1">
+    <row r="100" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A100" s="2" t="s">
         <v>365</v>
       </c>
@@ -36825,7 +36821,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.75" customHeight="1">
+    <row r="101" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A101" s="2" t="s">
         <v>387</v>
       </c>
@@ -36839,7 +36835,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.75" customHeight="1">
+    <row r="102" spans="1:4" ht="15.75" hidden="1" customHeight="1">
       <c r="A102" s="2" t="s">
         <v>388</v>
       </c>
@@ -38099,7 +38095,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="192" spans="1:4" ht="15.75" customHeight="1">
       <c r="A192" s="2" t="s">
         <v>583</v>
       </c>
@@ -38113,7 +38109,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="193" spans="1:4" ht="15.75" customHeight="1">
       <c r="A193" s="2" t="s">
         <v>584</v>
       </c>
@@ -38127,7 +38123,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="194" spans="1:4" ht="15.75" customHeight="1">
       <c r="A194" s="2" t="s">
         <v>585</v>
       </c>
@@ -38141,7 +38137,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="195" spans="1:4" ht="15.75" customHeight="1">
       <c r="A195" s="2" t="s">
         <v>588</v>
       </c>
@@ -38155,7 +38151,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="196" spans="1:4" ht="15.75" customHeight="1">
       <c r="A196" s="2" t="s">
         <v>559</v>
       </c>
@@ -38169,7 +38165,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="197" spans="1:4" ht="15.75" customHeight="1">
       <c r="A197" s="2" t="s">
         <v>579</v>
       </c>
@@ -38183,7 +38179,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="198" spans="1:4" ht="15.75" customHeight="1">
       <c r="A198" s="2" t="s">
         <v>615</v>
       </c>
@@ -38197,7 +38193,7 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="199" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="199" spans="1:4" ht="15.75" customHeight="1">
       <c r="A199" s="2" t="s">
         <v>619</v>
       </c>
@@ -38211,7 +38207,7 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="200" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="200" spans="1:4" ht="15.75" customHeight="1">
       <c r="A200" s="2" t="s">
         <v>604</v>
       </c>
@@ -38225,7 +38221,7 @@
         <v>1690</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="201" spans="1:4" ht="15.75" customHeight="1">
       <c r="A201" s="2" t="s">
         <v>605</v>
       </c>
@@ -38239,7 +38235,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="202" spans="1:4" ht="30" hidden="1">
+    <row r="202" spans="1:4" ht="30">
       <c r="A202" s="2" t="s">
         <v>601</v>
       </c>
@@ -38253,7 +38249,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="203" spans="1:4" ht="135" hidden="1">
+    <row r="203" spans="1:4" ht="135">
       <c r="A203" s="2" t="s">
         <v>582</v>
       </c>
@@ -38267,7 +38263,7 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="204" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="204" spans="1:4" ht="15.75" customHeight="1">
       <c r="A204" s="2" t="s">
         <v>657</v>
       </c>
@@ -38281,7 +38277,7 @@
         <v>1443</v>
       </c>
     </row>
-    <row r="205" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="205" spans="1:4" ht="15.75" customHeight="1">
       <c r="A205" s="2" t="s">
         <v>664</v>
       </c>
@@ -38295,7 +38291,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="206" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="206" spans="1:4" ht="15.75" customHeight="1">
       <c r="A206" s="2" t="s">
         <v>608</v>
       </c>
@@ -38309,7 +38305,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="207" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="207" spans="1:4" ht="15.75" customHeight="1">
       <c r="A207" s="2" t="s">
         <v>631</v>
       </c>
@@ -38323,7 +38319,7 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="208" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="208" spans="1:4" ht="15.75" customHeight="1">
       <c r="A208" s="2" t="s">
         <v>609</v>
       </c>
@@ -38337,7 +38333,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="209" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="209" spans="1:4" ht="15.75" customHeight="1">
       <c r="A209" s="2" t="s">
         <v>612</v>
       </c>
@@ -38351,7 +38347,7 @@
         <v>1453</v>
       </c>
     </row>
-    <row r="210" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="210" spans="1:4" ht="15.75" customHeight="1">
       <c r="A210" s="2" t="s">
         <v>634</v>
       </c>
@@ -38365,7 +38361,7 @@
         <v>1688</v>
       </c>
     </row>
-    <row r="211" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="211" spans="1:4" ht="15.75" customHeight="1">
       <c r="A211" s="2" t="s">
         <v>638</v>
       </c>
@@ -38379,7 +38375,7 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="212" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="212" spans="1:4" ht="15.75" customHeight="1">
       <c r="A212" s="2" t="s">
         <v>628</v>
       </c>
@@ -38393,7 +38389,7 @@
         <v>1458</v>
       </c>
     </row>
-    <row r="213" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="213" spans="1:4" ht="15.75" customHeight="1">
       <c r="A213" s="2" t="s">
         <v>598</v>
       </c>
@@ -38407,7 +38403,7 @@
         <v>1686</v>
       </c>
     </row>
-    <row r="214" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="214" spans="1:4" ht="15.75" customHeight="1">
       <c r="A214" s="2" t="s">
         <v>660</v>
       </c>
@@ -38421,7 +38417,7 @@
         <v>1461</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="215" spans="1:4" ht="15.75" customHeight="1">
       <c r="A215" s="2" t="s">
         <v>594</v>
       </c>
@@ -38435,7 +38431,7 @@
         <v>1463</v>
       </c>
     </row>
-    <row r="216" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="216" spans="1:4" ht="15.75" customHeight="1">
       <c r="A216" s="2" t="s">
         <v>622</v>
       </c>
@@ -38449,7 +38445,7 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="217" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="217" spans="1:4" ht="15.75" customHeight="1">
       <c r="A217" s="2" t="s">
         <v>597</v>
       </c>
@@ -38463,7 +38459,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="218" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="218" spans="1:4" ht="15.75" customHeight="1">
       <c r="A218" s="2" t="s">
         <v>667</v>
       </c>
@@ -38477,7 +38473,7 @@
         <v>1687</v>
       </c>
     </row>
-    <row r="219" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="219" spans="1:4" ht="15.75" customHeight="1">
       <c r="A219" s="2" t="s">
         <v>589</v>
       </c>
@@ -38491,7 +38487,7 @@
         <v>1470</v>
       </c>
     </row>
-    <row r="220" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="220" spans="1:4" ht="15.75" customHeight="1">
       <c r="A220" s="2" t="s">
         <v>590</v>
       </c>
@@ -38505,7 +38501,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="221" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="221" spans="1:4" ht="15.75" customHeight="1">
       <c r="A221" s="2" t="s">
         <v>653</v>
       </c>
@@ -38519,7 +38515,7 @@
         <v>1474</v>
       </c>
     </row>
-    <row r="222" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="222" spans="1:4" ht="15.75" customHeight="1">
       <c r="A222" s="2" t="s">
         <v>647</v>
       </c>
@@ -38533,7 +38529,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="223" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="223" spans="1:4" ht="15.75" customHeight="1">
       <c r="A223" s="2" t="s">
         <v>644</v>
       </c>
@@ -38547,7 +38543,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="224" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="224" spans="1:4" ht="15.75" customHeight="1">
       <c r="A224" s="2" t="s">
         <v>595</v>
       </c>
@@ -38561,7 +38557,7 @@
         <v>1689</v>
       </c>
     </row>
-    <row r="225" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="225" spans="1:4" ht="15.75" customHeight="1">
       <c r="A225" s="2" t="s">
         <v>591</v>
       </c>
@@ -38575,7 +38571,7 @@
         <v>1481</v>
       </c>
     </row>
-    <row r="226" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="226" spans="1:4" ht="15.75" customHeight="1">
       <c r="A226" s="2" t="s">
         <v>557</v>
       </c>
@@ -38589,7 +38585,7 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="227" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="227" spans="1:4" ht="15.75" customHeight="1">
       <c r="A227" s="2" t="s">
         <v>556</v>
       </c>
@@ -38603,7 +38599,7 @@
         <v>1484</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="228" spans="1:4" ht="15.75" customHeight="1">
       <c r="A228" s="2" t="s">
         <v>553</v>
       </c>
@@ -38617,7 +38613,7 @@
         <v>1486</v>
       </c>
     </row>
-    <row r="229" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="229" spans="1:4" ht="15.75" customHeight="1">
       <c r="A229" s="2" t="s">
         <v>555</v>
       </c>
@@ -38631,7 +38627,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="230" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="230" spans="1:4" ht="15.75" customHeight="1">
       <c r="A230" s="2" t="s">
         <v>568</v>
       </c>
@@ -38645,7 +38641,7 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="231" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="231" spans="1:4" ht="15.75" customHeight="1">
       <c r="A231" s="2" t="s">
         <v>571</v>
       </c>
@@ -38659,7 +38655,7 @@
         <v>1492</v>
       </c>
     </row>
-    <row r="232" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="232" spans="1:4" ht="15.75" customHeight="1">
       <c r="A232" s="2" t="s">
         <v>562</v>
       </c>
@@ -38673,7 +38669,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="233" spans="1:4" ht="15.75" customHeight="1">
       <c r="A233" s="2" t="s">
         <v>565</v>
       </c>
@@ -38687,7 +38683,7 @@
         <v>1495</v>
       </c>
     </row>
-    <row r="234" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="234" spans="1:4" ht="15.75" customHeight="1">
       <c r="A234" s="2" t="s">
         <v>576</v>
       </c>
@@ -38701,7 +38697,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="235" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="235" spans="1:4" ht="15.75" customHeight="1">
       <c r="A235" s="2" t="s">
         <v>573</v>
       </c>
@@ -38715,7 +38711,7 @@
         <v>1499</v>
       </c>
     </row>
-    <row r="236" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="236" spans="1:4" ht="15.75" customHeight="1">
       <c r="A236" s="2" t="s">
         <v>572</v>
       </c>
@@ -38729,7 +38725,7 @@
         <v>1501</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="237" spans="1:4" ht="15.75" customHeight="1">
       <c r="A237" s="2" t="s">
         <v>554</v>
       </c>
@@ -38743,7 +38739,7 @@
         <v>1503</v>
       </c>
     </row>
-    <row r="238" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="238" spans="1:4" ht="15.75" customHeight="1">
       <c r="A238" s="2" t="s">
         <v>641</v>
       </c>
@@ -38757,7 +38753,7 @@
         <v>1505</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="45" hidden="1">
+    <row r="239" spans="1:4" ht="45">
       <c r="A239" s="2" t="s">
         <v>650</v>
       </c>
@@ -38771,7 +38767,7 @@
         <v>1507</v>
       </c>
     </row>
-    <row r="240" spans="1:4" ht="15.75" hidden="1" customHeight="1">
+    <row r="240" spans="1:4" ht="15.75" customHeight="1">
       <c r="A240" s="2" t="s">
         <v>625</v>
       </c>
@@ -40258,52 +40254,55 @@
   <autoFilter ref="A1:H310" xr:uid="{00000000-0009-0000-0000-000006000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="ADLBC.A1HI"/>
-        <filter val="ADLBC.A1LO"/>
-        <filter val="ADLBC.ABLFL"/>
-        <filter val="ADLBC.ADT"/>
-        <filter val="ADLBC.ADY"/>
-        <filter val="ADLBC.AENTMTFL"/>
-        <filter val="ADLBC.AGE"/>
-        <filter val="ADLBC.AGEGR1"/>
-        <filter val="ADLBC.AGEGR1N"/>
-        <filter val="ADLBC.ALBTRVAL"/>
-        <filter val="ADLBC.ANL01FL"/>
-        <filter val="ADLBC.ANRIND"/>
-        <filter val="ADLBC.AVAL"/>
-        <filter val="ADLBC.AVISIT"/>
-        <filter val="ADLBC.AVISITN"/>
-        <filter val="ADLBC.BASE"/>
-        <filter val="ADLBC.BNRIND"/>
-        <filter val="ADLBC.BR2A1HI"/>
-        <filter val="ADLBC.BR2A1LO"/>
-        <filter val="ADLBC.CHG"/>
-        <filter val="ADLBC.COMP24FL"/>
-        <filter val="ADLBC.DSRAEFL"/>
-        <filter val="ADLBC.LBNRIND"/>
-        <filter val="ADLBC.LBSEQ"/>
-        <filter val="ADLBC.LBSTRESN"/>
-        <filter val="ADLBC.PARAM"/>
-        <filter val="ADLBC.PARAMCD"/>
-        <filter val="ADLBC.PARAMN"/>
-        <filter val="ADLBC.PARCAT1"/>
-        <filter val="ADLBC.R2A1HI"/>
-        <filter val="ADLBC.R2A1LO"/>
-        <filter val="ADLBC.RACE"/>
-        <filter val="ADLBC.RACEN"/>
-        <filter val="ADLBC.SAFFL"/>
-        <filter val="ADLBC.SEX"/>
-        <filter val="ADLBC.STUDYID"/>
-        <filter val="ADLBC.SUBJID"/>
-        <filter val="ADLBC.TRTA"/>
-        <filter val="ADLBC.TRTAN"/>
-        <filter val="ADLBC.TRTEDT"/>
-        <filter val="ADLBC.TRTP"/>
-        <filter val="ADLBC.TRTPN"/>
-        <filter val="ADLBC.TRTSDT"/>
-        <filter val="ADLBC.USUBJID"/>
-        <filter val="ADLBC.VISIT"/>
-        <filter val="ADLBC.VISITNUM"/>
+        <filter val="ADSL.AGE"/>
+        <filter val="ADSL.AGEGR1"/>
+        <filter val="ADSL.AGEGR1N"/>
+        <filter val="ADSL.AGEU"/>
+        <filter val="ADSL.ARM"/>
+        <filter val="ADSL.AVGDD"/>
+        <filter val="ADSL.BMIBL"/>
+        <filter val="ADSL.BMIBLGR1"/>
+        <filter val="ADSL.COMP16FL"/>
+        <filter val="ADSL.COMP24FL"/>
+        <filter val="ADSL.COMP8FL"/>
+        <filter val="ADSL.CUMDOSE"/>
+        <filter val="ADSL.DCDECOD"/>
+        <filter val="ADSL.DCREASCD"/>
+        <filter val="ADSL.DISCONFL"/>
+        <filter val="ADSL.DISONSDT"/>
+        <filter val="ADSL.DSRAEFL"/>
+        <filter val="ADSL.DTHFL"/>
+        <filter val="ADSL.DURDIS"/>
+        <filter val="ADSL.DURDSGR1"/>
+        <filter val="ADSL.EDUCLVL"/>
+        <filter val="ADSL.EFFFL"/>
+        <filter val="ADSL.EOSSTT"/>
+        <filter val="ADSL.ETHNIC"/>
+        <filter val="ADSL.HEIGHTBL"/>
+        <filter val="ADSL.ITTFL"/>
+        <filter val="ADSL.MMSETOT"/>
+        <filter val="ADSL.RACE"/>
+        <filter val="ADSL.RACEN"/>
+        <filter val="ADSL.RFENDT"/>
+        <filter val="ADSL.RFENDTC"/>
+        <filter val="ADSL.RFSTDTC"/>
+        <filter val="ADSL.SAFFL"/>
+        <filter val="ADSL.SEX"/>
+        <filter val="ADSL.SITEGR1"/>
+        <filter val="ADSL.SITEID"/>
+        <filter val="ADSL.STUDYID"/>
+        <filter val="ADSL.SUBJID"/>
+        <filter val="ADSL.TRT01A"/>
+        <filter val="ADSL.TRT01AN"/>
+        <filter val="ADSL.TRT01P"/>
+        <filter val="ADSL.TRT01PN"/>
+        <filter val="ADSL.TRTDUR"/>
+        <filter val="ADSL.TRTEDT"/>
+        <filter val="ADSL.TRTSDT"/>
+        <filter val="ADSL.USUBJID"/>
+        <filter val="ADSL.VISIT1DT"/>
+        <filter val="ADSL.VISNUMEN"/>
+        <filter val="ADSL.WEIGHTBL"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>